<commit_message>
Various updates, especially concerning subject/course data.
</commit_message>
<xml_diff>
--- a/TESTDATA/RESOURCES/templates/Fachwahl.xlsx
+++ b/TESTDATA/RESOURCES/templates/Fachwahl.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="13">
-  <si>
-    <t xml:space="preserve">#</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="12">
   <si>
     <t xml:space="preserve">Fächerwahl</t>
   </si>
@@ -340,10 +337,10 @@
   <dimension ref="A1:AD1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8:C49"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.74"/>
@@ -355,11 +352,9 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -380,18 +375,18 @@
     </row>
     <row r="2" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>4</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -411,13 +406,13 @@
     </row>
     <row r="3" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>7</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -440,97 +435,97 @@
     <row r="4" customFormat="false" ht="8.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="44.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="C5" s="9" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>10</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="T5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="U5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="V5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="W5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="X5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AA5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AB5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AC5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AD5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="94.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -596,7 +591,7 @@
     </row>
     <row r="8" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="15"/>
@@ -630,7 +625,7 @@
     </row>
     <row r="9" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -664,7 +659,7 @@
     </row>
     <row r="10" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="15"/>
@@ -698,7 +693,7 @@
     </row>
     <row r="11" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="15"/>
@@ -732,7 +727,7 @@
     </row>
     <row r="12" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="15"/>
@@ -766,7 +761,7 @@
     </row>
     <row r="13" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="15"/>
@@ -800,7 +795,7 @@
     </row>
     <row r="14" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="15"/>
@@ -834,7 +829,7 @@
     </row>
     <row r="15" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="15"/>
@@ -868,7 +863,7 @@
     </row>
     <row r="16" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="15"/>
@@ -902,7 +897,7 @@
     </row>
     <row r="17" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
@@ -936,7 +931,7 @@
     </row>
     <row r="18" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
@@ -970,7 +965,7 @@
     </row>
     <row r="19" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
@@ -1004,7 +999,7 @@
     </row>
     <row r="20" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="15"/>
@@ -1038,7 +1033,7 @@
     </row>
     <row r="21" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
@@ -1072,7 +1067,7 @@
     </row>
     <row r="22" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
@@ -1106,7 +1101,7 @@
     </row>
     <row r="23" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
@@ -1140,7 +1135,7 @@
     </row>
     <row r="24" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
@@ -1174,7 +1169,7 @@
     </row>
     <row r="25" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -1208,7 +1203,7 @@
     </row>
     <row r="26" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
@@ -1242,7 +1237,7 @@
     </row>
     <row r="27" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
@@ -1276,7 +1271,7 @@
     </row>
     <row r="28" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
@@ -1310,7 +1305,7 @@
     </row>
     <row r="29" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>
@@ -1344,7 +1339,7 @@
     </row>
     <row r="30" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30" s="14"/>
       <c r="C30" s="15"/>
@@ -1378,7 +1373,7 @@
     </row>
     <row r="31" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31" s="14"/>
       <c r="C31" s="15"/>
@@ -1412,7 +1407,7 @@
     </row>
     <row r="32" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1446,7 +1441,7 @@
     </row>
     <row r="33" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B33" s="14"/>
       <c r="C33" s="15"/>
@@ -1480,7 +1475,7 @@
     </row>
     <row r="34" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B34" s="14"/>
       <c r="C34" s="15"/>
@@ -1514,7 +1509,7 @@
     </row>
     <row r="35" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B35" s="14"/>
       <c r="C35" s="15"/>
@@ -1548,7 +1543,7 @@
     </row>
     <row r="36" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B36" s="14"/>
       <c r="C36" s="15"/>
@@ -1582,7 +1577,7 @@
     </row>
     <row r="37" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B37" s="14"/>
       <c r="C37" s="15"/>
@@ -1616,7 +1611,7 @@
     </row>
     <row r="38" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B38" s="14"/>
       <c r="C38" s="15"/>
@@ -1650,7 +1645,7 @@
     </row>
     <row r="39" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B39" s="14"/>
       <c r="C39" s="15"/>
@@ -1684,7 +1679,7 @@
     </row>
     <row r="40" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B40" s="14"/>
       <c r="C40" s="15"/>
@@ -1718,7 +1713,7 @@
     </row>
     <row r="41" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B41" s="14"/>
       <c r="C41" s="15"/>
@@ -1752,7 +1747,7 @@
     </row>
     <row r="42" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B42" s="14"/>
       <c r="C42" s="15"/>
@@ -1786,7 +1781,7 @@
     </row>
     <row r="43" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B43" s="14"/>
       <c r="C43" s="15"/>
@@ -1820,7 +1815,7 @@
     </row>
     <row r="44" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B44" s="14"/>
       <c r="C44" s="15"/>
@@ -1854,7 +1849,7 @@
     </row>
     <row r="45" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B45" s="14"/>
       <c r="C45" s="15"/>
@@ -1888,7 +1883,7 @@
     </row>
     <row r="46" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B46" s="14"/>
       <c r="C46" s="15"/>
@@ -1922,7 +1917,7 @@
     </row>
     <row r="47" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B47" s="14"/>
       <c r="C47" s="15"/>
@@ -1956,7 +1951,7 @@
     </row>
     <row r="48" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B48" s="14"/>
       <c r="C48" s="15"/>
@@ -1990,7 +1985,7 @@
     </row>
     <row r="49" customFormat="false" ht="22.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49" s="14"/>
       <c r="C49" s="15"/>
@@ -2036,14 +2031,14 @@
     <mergeCell ref="R3:S3"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E8:AD49" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E8:AD49" type="list">
       <formula1>"/"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.636805555555555" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>